<commit_message>
Updating file upload method.
</commit_message>
<xml_diff>
--- a/uploadedTemplates/template_testUpload_inconsistentTags.xlsx
+++ b/uploadedTemplates/template_testUpload_inconsistentTags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/uploadedTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9825487C-80DA-B147-90D4-2ABE41F65264}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A20AEC-B459-7242-BCBE-C44F82C4833C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="24700" windowHeight="11360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="500" windowWidth="24700" windowHeight="11360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="studies" sheetId="1" r:id="rId1"/>
@@ -321,7 +321,7 @@
     <t>beats/min increase</t>
   </si>
   <si>
-    <t>hrate_variability_fake</t>
+    <t>pocok</t>
   </si>
 </sst>
 </file>
@@ -923,7 +923,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>